<commit_message>
Clase de equivalencia compra billete rematada
</commit_message>
<xml_diff>
--- a/Juan_G/compra_billete_2/clases_equivalencia.xlsx
+++ b/Juan_G/compra_billete_2/clases_equivalencia.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="208" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="208"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Hoja3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -113,7 +112,7 @@
     <t>Adultos</t>
   </si>
   <si>
-    <t>Obligatorio </t>
+    <t>Obligatorio</t>
   </si>
   <si>
     <t>17: Número entre 0 y 9</t>
@@ -155,51 +154,33 @@
     <t>Cód Promo</t>
   </si>
   <si>
-    <t>26: Todo alfanumérico que sea un código válido</t>
-  </si>
-  <si>
-    <t>27: Todo alfanumérico que sea un código NO válido</t>
+    <t>26: Todo alfanumérico que sea un código válido 27: Vacio</t>
+  </si>
+  <si>
+    <t>28: Todo alfanumérico que sea un código NO válido</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <family val="2"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
+      <i/>
       <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="true"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <i val="true"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -211,7 +192,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -219,79 +200,342 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B15" activeCellId="0" pane="topLeft" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3490196078431"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.643137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.0705882352941"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5764705882353"/>
+    <col min="1" max="1" width="34.28515625"/>
+    <col min="2" max="2" width="21.85546875"/>
+    <col min="3" max="3" width="33.5703125"/>
+    <col min="4" max="4" width="34"/>
+    <col min="5" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="1">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -305,22 +549,22 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -330,11 +574,11 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -344,25 +588,25 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -372,25 +616,25 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -400,69 +644,69 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="10">
+    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="12">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="13">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="14">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -473,10 +717,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
   </headerFooter>
@@ -484,24 +727,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col min="1" max="1025" width="11.5703125"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
   </headerFooter>
@@ -509,24 +746,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col min="1" max="1025" width="11.5703125"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
   </headerFooter>

</xml_diff>